<commit_message>
Fix supplier table: break out Avnet family, only combine Abacus+Silica
</commit_message>
<xml_diff>
--- a/Trading Analysis/LAM review/LAM NewParts - Summary Tables.xlsx
+++ b/Trading Analysis/LAM review/LAM NewParts - Summary Tables.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -483,6 +483,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
@@ -652,6 +653,7 @@
         </is>
       </c>
     </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
@@ -861,6 +863,7 @@
         </is>
       </c>
     </row>
+    <row r="23"/>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
@@ -1235,6 +1238,7 @@
         </is>
       </c>
     </row>
+    <row r="36"/>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
@@ -1296,6 +1300,7 @@
         <v>6</v>
       </c>
     </row>
+    <row r="43"/>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
@@ -1393,6 +1398,8 @@
         </is>
       </c>
     </row>
+    <row r="50"/>
+    <row r="51"/>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
@@ -1715,39 +1722,39 @@
     <row r="65">
       <c r="A65" s="6" t="inlineStr">
         <is>
-          <t>Future</t>
+          <t>Avnet Abacus/Silica</t>
         </is>
       </c>
       <c r="B65" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D65" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F65" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G65" s="6" t="n">
         <v>3</v>
-      </c>
-      <c r="C65" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D65" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E65" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F65" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" s="6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="6" t="inlineStr">
         <is>
-          <t>Schukat</t>
+          <t>Future</t>
         </is>
       </c>
       <c r="B66" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66" s="6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D66" s="6" t="n">
         <v>3</v>
@@ -1756,7 +1763,7 @@
         <v>3</v>
       </c>
       <c r="F66" s="6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G66" s="6" t="n">
         <v>1</v>
@@ -1765,14 +1772,14 @@
     <row r="67">
       <c r="A67" s="6" t="inlineStr">
         <is>
-          <t>AvnetAbacus</t>
+          <t>Schukat</t>
         </is>
       </c>
       <c r="B67" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" s="6" t="n">
         <v>2</v>
-      </c>
-      <c r="C67" s="6" t="n">
-        <v>1</v>
       </c>
       <c r="D67" s="6" t="n">
         <v>3</v>
@@ -1781,10 +1788,10 @@
         <v>3</v>
       </c>
       <c r="F67" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G67" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1840,7 +1847,7 @@
     <row r="70">
       <c r="A70" s="6" t="inlineStr">
         <is>
-          <t>AvnetSilica</t>
+          <t>Rutronik</t>
         </is>
       </c>
       <c r="B70" s="6" t="n">
@@ -1865,53 +1872,38 @@
     <row r="71">
       <c r="A71" s="6" t="inlineStr">
         <is>
-          <t>Rutronik</t>
+          <t>Unknown (no supplier)</t>
         </is>
       </c>
       <c r="B71" s="6" t="n">
+        <v>80</v>
+      </c>
+      <c r="C71" s="6" t="n">
+        <v>106</v>
+      </c>
+      <c r="D71" s="6" t="n">
+        <v>186</v>
+      </c>
+      <c r="E71" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C71" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D71" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E71" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="F71" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="6" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="B72" s="6" t="n">
-        <v>80</v>
-      </c>
-      <c r="C72" s="6" t="n">
-        <v>106</v>
-      </c>
-      <c r="D72" s="6" t="n">
-        <v>186</v>
-      </c>
-      <c r="E72" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" s="6" t="n">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="A72" s="6" t="n"/>
+      <c r="B72" s="6" t="n"/>
+      <c r="C72" s="6" t="n"/>
+      <c r="D72" s="6" t="n"/>
+      <c r="E72" s="6" t="n"/>
+      <c r="F72" s="6" t="n"/>
+      <c r="G72" s="6" t="n"/>
+    </row>
+    <row r="73"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>